<commit_message>
updated powerBI dashboard adding filters and buttons
</commit_message>
<xml_diff>
--- a/PowerBI data/Combined data.xlsx
+++ b/PowerBI data/Combined data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antho\OneDrive\Documents\AB course\powerBI-Assessment\PowerBI data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{FEFD33F5-B74E-4E67-A6D8-8561D7EF1A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD01D79-8EE5-4BD0-9156-BA39F8A1D0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9390EF0D-E8AC-4EF4-9AA6-705A206F08D8}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">'GDP per capita growth (annual %'!$A:$BP</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2748" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2747" uniqueCount="746">
   <si>
     <t/>
   </si>
@@ -2306,9 +2305,6 @@
   </si>
   <si>
     <t>E. Asia and Pacific</t>
-  </si>
-  <si>
-    <t>Average</t>
   </si>
   <si>
     <t>N. America</t>
@@ -2343,7 +2339,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2356,14 +2352,8 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2419,35 +2409,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2455,23 +2432,22 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2607,6 +2583,9 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2683,10 +2662,23 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -2703,21 +2695,6 @@
           <color theme="9" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2750,29 +2727,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C9B92E62-2639-43A6-A2F3-AA916821C1C9}" name="Table6" displayName="Table6" ref="B4:U68" totalsRowShown="0">
-  <autoFilter ref="B4:U68" xr:uid="{C9B92E62-2639-43A6-A2F3-AA916821C1C9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C9B92E62-2639-43A6-A2F3-AA916821C1C9}" name="Table6" displayName="Table6" ref="B4:U67" totalsRowShown="0">
+  <autoFilter ref="B4:U67" xr:uid="{C9B92E62-2639-43A6-A2F3-AA916821C1C9}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{DC068CCD-FD40-4A05-BCD5-FC8A7A5C9AF7}" name="Year"/>
-    <tableColumn id="2" xr3:uid="{8E3DA648-100E-4812-B56F-2036EB6755AE}" name="UK " dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{2D81A98B-A52D-4C97-A1E7-569800F36438}" name="US " dataDxfId="14" dataCellStyle="Percent"/>
-    <tableColumn id="9" xr3:uid="{72597C87-D6AE-466F-98C4-9F487BAA61A9}" name="France " dataDxfId="11" dataCellStyle="Percent"/>
-    <tableColumn id="13" xr3:uid="{B23F1DB5-C280-437E-9CA3-A52AE8426CCC}" name="Germany " dataDxfId="8" dataCellStyle="Percent"/>
-    <tableColumn id="14" xr3:uid="{1014762B-7B5A-4C25-B5B2-D98E8A551E63}" name="Canada " dataDxfId="6" dataCellStyle="Percent"/>
-    <tableColumn id="15" xr3:uid="{E7C5170E-EA9D-4712-B0E4-366B6D9AC398}" name="Italy " dataDxfId="7" dataCellStyle="Percent"/>
-    <tableColumn id="10" xr3:uid="{7A8DE665-0EE7-40E5-9D0B-5B2876F34CF3}" name="Japan " dataDxfId="10" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{8E3DA648-100E-4812-B56F-2036EB6755AE}" name="UK " dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{2D81A98B-A52D-4C97-A1E7-569800F36438}" name="US " dataDxfId="19" dataCellStyle="Percent"/>
+    <tableColumn id="9" xr3:uid="{72597C87-D6AE-466F-98C4-9F487BAA61A9}" name="France " dataDxfId="18" dataCellStyle="Percent"/>
+    <tableColumn id="13" xr3:uid="{B23F1DB5-C280-437E-9CA3-A52AE8426CCC}" name="Germany " dataDxfId="17" dataCellStyle="Percent"/>
+    <tableColumn id="14" xr3:uid="{1014762B-7B5A-4C25-B5B2-D98E8A551E63}" name="Canada " dataDxfId="16" dataCellStyle="Percent"/>
+    <tableColumn id="15" xr3:uid="{E7C5170E-EA9D-4712-B0E4-366B6D9AC398}" name="Italy " dataDxfId="15" dataCellStyle="Percent"/>
+    <tableColumn id="10" xr3:uid="{7A8DE665-0EE7-40E5-9D0B-5B2876F34CF3}" name="Japan " dataDxfId="14" dataCellStyle="Percent"/>
     <tableColumn id="4" xr3:uid="{F5131250-3A70-4A52-8FC8-B73ACB191D13}" name="Brazil " dataDxfId="13" dataCellStyle="Percent"/>
     <tableColumn id="5" xr3:uid="{76E249FB-7FBB-4E4C-A7F8-8572FC054696}" name="Russia "/>
     <tableColumn id="6" xr3:uid="{C631BCA8-769A-41FA-99C5-E81538810CE1}" name="India "/>
     <tableColumn id="7" xr3:uid="{3CD0D7A7-945B-428E-9332-2E77489538AE}" name="China "/>
-    <tableColumn id="16" xr3:uid="{E56BF660-368E-4CD2-B7D8-C7B4226F6423}" name="Sub Saharan Africa " dataDxfId="5" dataCellStyle="Percent"/>
-    <tableColumn id="17" xr3:uid="{EF99D586-8F71-420A-851B-F1A1F7DA9D59}" name="N. Africa and Mid. East" dataDxfId="4" dataCellStyle="Percent"/>
-    <tableColumn id="18" xr3:uid="{085E04AF-B9A4-4E68-A1D6-BDF6794F90EB}" name="Latin A. and Carib. " dataDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="20" xr3:uid="{140D63C5-3F1C-441F-B0C8-C74C60CA5C1C}" name="E. Asia and Pacific" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="19" xr3:uid="{7A1F1F94-A494-4D97-9324-95F30FE454CD}" name="Europe and C.Asia" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="21" xr3:uid="{08DEDB35-93E3-4E36-923C-A13ACE60D485}" name="N. America" dataDxfId="0" dataCellStyle="Percent"/>
-    <tableColumn id="12" xr3:uid="{C6B5A247-A040-4D31-B073-EA7963B21DC9}" name="EU" dataDxfId="9" dataCellStyle="Percent"/>
-    <tableColumn id="8" xr3:uid="{1BA06C18-99BF-4B7F-A228-9FDF0007076B}" name="World GDP" dataDxfId="12">
+    <tableColumn id="16" xr3:uid="{E56BF660-368E-4CD2-B7D8-C7B4226F6423}" name="Sub Saharan Africa " dataDxfId="12" dataCellStyle="Percent"/>
+    <tableColumn id="17" xr3:uid="{EF99D586-8F71-420A-851B-F1A1F7DA9D59}" name="N. Africa and Mid. East" dataDxfId="11" dataCellStyle="Percent"/>
+    <tableColumn id="18" xr3:uid="{085E04AF-B9A4-4E68-A1D6-BDF6794F90EB}" name="Latin A. and Carib. " dataDxfId="10" dataCellStyle="Percent"/>
+    <tableColumn id="20" xr3:uid="{140D63C5-3F1C-441F-B0C8-C74C60CA5C1C}" name="E. Asia and Pacific" dataDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="19" xr3:uid="{7A1F1F94-A494-4D97-9324-95F30FE454CD}" name="Europe and C.Asia" dataDxfId="8" dataCellStyle="Percent"/>
+    <tableColumn id="21" xr3:uid="{08DEDB35-93E3-4E36-923C-A13ACE60D485}" name="N. America" dataDxfId="7" dataCellStyle="Percent"/>
+    <tableColumn id="12" xr3:uid="{C6B5A247-A040-4D31-B073-EA7963B21DC9}" name="EU" dataDxfId="6" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{1BA06C18-99BF-4B7F-A228-9FDF0007076B}" name="World GDP" dataDxfId="5">
       <calculatedColumnFormula>M5/100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2867,11 +2844,11 @@
     <sortCondition ref="B1:B266"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CF0B21A7-5FBF-460F-8CB2-AD367B90B065}" uniqueName="1" name="Country Code" queryTableFieldId="1" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{99F564E0-76B3-4E4F-A65F-BB0EC54929EC}" uniqueName="2" name="Region" queryTableFieldId="2" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{C37AD297-6C08-42C0-9A75-7DC99EE34E2F}" uniqueName="3" name="IncomeGroup" queryTableFieldId="3" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{E4BBB2F2-F767-4DE8-9B74-5A51ADE6E7C9}" uniqueName="4" name="SpecialNotes" queryTableFieldId="4" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{F5C95105-D299-46FB-95C0-A9ADB58534B2}" uniqueName="5" name="TableName" queryTableFieldId="5" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{CF0B21A7-5FBF-460F-8CB2-AD367B90B065}" uniqueName="1" name="Country Code" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{99F564E0-76B3-4E4F-A65F-BB0EC54929EC}" uniqueName="2" name="Region" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{C37AD297-6C08-42C0-9A75-7DC99EE34E2F}" uniqueName="3" name="IncomeGroup" queryTableFieldId="3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{E4BBB2F2-F767-4DE8-9B74-5A51ADE6E7C9}" uniqueName="4" name="SpecialNotes" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{F5C95105-D299-46FB-95C0-A9ADB58534B2}" uniqueName="5" name="TableName" queryTableFieldId="5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3174,10 +3151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F87BB86-D23A-4D69-88EB-A89080B5874C}">
-  <dimension ref="B4:Y68"/>
+  <dimension ref="B4:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3254,7 +3231,7 @@
         <v>727</v>
       </c>
       <c r="S4" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="T4" t="s">
         <v>728</v>
@@ -7069,87 +7046,6 @@
       </c>
       <c r="U67" s="8">
         <v>2.2637292918766996E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B68" s="10" t="s">
-        <v>745</v>
-      </c>
-      <c r="C68" s="11">
-        <f>SUM(C6:C67)/COUNT(C6:C67)</f>
-        <v>1.9160322831122043E-2</v>
-      </c>
-      <c r="D68" s="11">
-        <f t="shared" ref="D68:U68" si="0">SUM(D6:D67)/COUNT(D6:D67)</f>
-        <v>1.9588661129832315E-2</v>
-      </c>
-      <c r="E68" s="11">
-        <f t="shared" si="0"/>
-        <v>2.0604185585694029E-2</v>
-      </c>
-      <c r="F68" s="11">
-        <f t="shared" si="0"/>
-        <v>1.7228261334159726E-2</v>
-      </c>
-      <c r="G68" s="11">
-        <f t="shared" si="0"/>
-        <v>1.5956689416731992E-2</v>
-      </c>
-      <c r="H68" s="11">
-        <f t="shared" si="0"/>
-        <v>2.0344503836623038E-2</v>
-      </c>
-      <c r="I68" s="11">
-        <f t="shared" si="0"/>
-        <v>2.9224302906149573E-2</v>
-      </c>
-      <c r="J68" s="11">
-        <f t="shared" si="0"/>
-        <v>2.0738566409674922E-2</v>
-      </c>
-      <c r="K68" s="11">
-        <f t="shared" si="0"/>
-        <v>9.2396194514342972E-3</v>
-      </c>
-      <c r="L68" s="11">
-        <f t="shared" si="0"/>
-        <v>3.1980394000037965E-2</v>
-      </c>
-      <c r="M68" s="11">
-        <f t="shared" si="0"/>
-        <v>6.6814748004898547E-2</v>
-      </c>
-      <c r="N68" s="11">
-        <f t="shared" si="0"/>
-        <v>6.0217279767718554E-3</v>
-      </c>
-      <c r="O68" s="11">
-        <f t="shared" si="0"/>
-        <v>7.5402075791793626E-3</v>
-      </c>
-      <c r="P68" s="11">
-        <f t="shared" si="0"/>
-        <v>4.2054277025322183E-2</v>
-      </c>
-      <c r="Q68" s="11">
-        <f t="shared" si="0"/>
-        <v>3.9374623542067361E-2</v>
-      </c>
-      <c r="R68" s="11">
-        <f t="shared" si="0"/>
-        <v>1.7147403944167413E-2</v>
-      </c>
-      <c r="S68" s="11">
-        <f t="shared" si="0"/>
-        <v>1.9129737028263892E-2</v>
-      </c>
-      <c r="T68" s="11">
-        <f t="shared" si="0"/>
-        <v>1.8401788755081815E-2</v>
-      </c>
-      <c r="U68" s="11">
-        <f t="shared" si="0"/>
-        <v>1.8691070307997829E-2</v>
       </c>
     </row>
   </sheetData>
@@ -7168,8 +7064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30853999-5130-4249-9661-5DFB99FB2AD3}">
   <dimension ref="A1:BP267"/>
   <sheetViews>
-    <sheetView topLeftCell="AZ161" workbookViewId="0">
-      <selection activeCell="G181" sqref="G181:BP181"/>
+    <sheetView topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BT194" sqref="BT194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50093,7 +49989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74141FD-1BF0-47B4-949C-998A61454FDF}">
   <dimension ref="A1:E266"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>